<commit_message>
First pass on all states
</commit_message>
<xml_diff>
--- a/docs/WIP/Maps & Elections by State.xlsx
+++ b/docs/WIP/Maps & Elections by State.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10706"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/dev/method_eval/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/dev/method_eval/docs/WIP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FADB8C-E483-8C4A-9BFC-3D381ADBBD45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59473D2-B9D4-0144-80D7-FB39DB1925FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="1060" windowWidth="27260" windowHeight="16940" xr2:uid="{681EA93E-AE60-7D46-B720-CAB4E15116B4}"/>
+    <workbookView xWindow="1080" yWindow="500" windowWidth="27720" windowHeight="17500" xr2:uid="{681EA93E-AE60-7D46-B720-CAB4E15116B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Elections by State" sheetId="2" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="196">
   <si>
     <t>AL</t>
   </si>
@@ -465,33 +465,18 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>TODO</t>
-  </si>
-  <si>
-    <t>Is "About Data" wrong re: P?</t>
-  </si>
-  <si>
-    <t>Which S2018?</t>
-  </si>
-  <si>
     <t>2021 elections</t>
   </si>
   <si>
     <t>Only one CD</t>
   </si>
   <si>
-    <t>No P2016, just P2012</t>
-  </si>
-  <si>
     <t>Only P elections; only two districts</t>
   </si>
   <si>
     <t>No AG election</t>
   </si>
   <si>
-    <t>AG2018 not *'d in "About Data"</t>
-  </si>
-  <si>
     <t>No AG election. Also S2018 not *'d in "About Data"</t>
   </si>
   <si>
@@ -666,7 +651,13 @@
     <t>117_D</t>
   </si>
   <si>
-    <t>Is this the latest?</t>
+    <t>AG2018 not contested.</t>
+  </si>
+  <si>
+    <t>No P2016, due to large Other vote.</t>
+  </si>
+  <si>
+    <t>We use the regular S2018, not the special or runoff.</t>
   </si>
 </sst>
 </file>
@@ -727,12 +718,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1051,13 +1043,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9549FD63-5553-FE4A-95C6-DE5AEB491F85}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N37" sqref="N37"/>
+      <selection pane="bottomRight" activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1092,7 +1085,7 @@
         <v>77</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>55</v>
@@ -1119,10 +1112,10 @@
         <v>58</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -1163,13 +1156,13 @@
         <v>6</v>
       </c>
       <c r="O2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="P2" s="4">
         <v>44721</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1192,7 +1185,7 @@
         <v>129</v>
       </c>
       <c r="N3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>130</v>
@@ -1236,7 +1229,7 @@
         <v>6</v>
       </c>
       <c r="O4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="P4" s="4">
         <v>44721</v>
@@ -1280,13 +1273,13 @@
         <v>6</v>
       </c>
       <c r="O5" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="P5" s="4">
         <v>44721</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1311,20 +1304,20 @@
       <c r="H6" t="s">
         <v>2</v>
       </c>
-      <c r="I6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" t="s">
         <v>6</v>
       </c>
       <c r="M6" t="s">
         <v>129</v>
       </c>
       <c r="N6" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="O6" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="P6" s="4">
         <v>44721</v>
@@ -1368,7 +1361,7 @@
         <v>6</v>
       </c>
       <c r="O7" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P7" s="4">
         <v>44721</v>
@@ -1412,19 +1405,16 @@
         <v>6</v>
       </c>
       <c r="M8" t="s">
-        <v>131</v>
-      </c>
-      <c r="N8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="O8" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="P8" s="4">
         <v>44721</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -1447,7 +1437,7 @@
         <v>129</v>
       </c>
       <c r="N9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="P9" s="4" t="s">
         <v>130</v>
@@ -1491,7 +1481,7 @@
         <v>6</v>
       </c>
       <c r="O10" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="P10" s="4">
         <v>44721</v>
@@ -1535,13 +1525,13 @@
         <v>6</v>
       </c>
       <c r="O11" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="P11" s="4">
         <v>44721</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1582,16 +1572,16 @@
         <v>129</v>
       </c>
       <c r="N12" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="O12" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="P12" s="4">
         <v>44721</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1632,10 +1622,10 @@
         <v>129</v>
       </c>
       <c r="N13" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="O13" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="P13" s="4">
         <v>44721</v>
@@ -1679,7 +1669,7 @@
         <v>6</v>
       </c>
       <c r="O14" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="P14" s="4">
         <v>44721</v>
@@ -1723,7 +1713,7 @@
         <v>23</v>
       </c>
       <c r="O15" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="P15" s="4">
         <v>44721</v>
@@ -1767,7 +1757,7 @@
         <v>6</v>
       </c>
       <c r="O16" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="P16" s="4">
         <v>44721</v>
@@ -1811,13 +1801,13 @@
         <v>6</v>
       </c>
       <c r="O17" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="P17" s="4">
         <v>44721</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1852,10 +1842,10 @@
         <v>129</v>
       </c>
       <c r="N18" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="O18" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="P18" s="4">
         <v>44721</v>
@@ -1899,16 +1889,16 @@
         <v>27</v>
       </c>
       <c r="N19" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="O19" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="P19" s="4">
         <v>44721</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1936,20 +1926,17 @@
       <c r="I20" t="s">
         <v>3</v>
       </c>
-      <c r="J20" t="s">
-        <v>5</v>
-      </c>
       <c r="K20" t="s">
-        <v>130</v>
+        <v>5</v>
       </c>
       <c r="M20" t="s">
         <v>129</v>
       </c>
       <c r="N20" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="O20" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="P20" s="4">
         <v>44721</v>
@@ -1993,7 +1980,7 @@
         <v>6</v>
       </c>
       <c r="O21" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="P21" s="4">
         <v>44721</v>
@@ -2037,7 +2024,7 @@
         <v>6</v>
       </c>
       <c r="O22" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="P22" s="4">
         <v>44721</v>
@@ -2081,7 +2068,7 @@
         <v>6</v>
       </c>
       <c r="O23" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="P23" s="4">
         <v>44721</v>
@@ -2125,13 +2112,13 @@
         <v>6</v>
       </c>
       <c r="M24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N24" t="s">
-        <v>133</v>
+        <v>195</v>
       </c>
       <c r="O24" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="P24" s="4">
         <v>44721</v>
@@ -2175,13 +2162,13 @@
         <v>27</v>
       </c>
       <c r="M25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N25" t="s">
-        <v>133</v>
+        <v>195</v>
       </c>
       <c r="O25" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="P25" s="4">
         <v>44721</v>
@@ -2225,13 +2212,13 @@
         <v>23</v>
       </c>
       <c r="O26" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="P26" s="4">
         <v>44721</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -2272,16 +2259,16 @@
         <v>129</v>
       </c>
       <c r="N27" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="O27" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="P27" s="4">
         <v>44721</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -2319,13 +2306,13 @@
         <v>6</v>
       </c>
       <c r="M28" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N28" t="s">
-        <v>139</v>
+        <v>193</v>
       </c>
       <c r="O28" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="P28" s="4">
         <v>44721</v>
@@ -2369,13 +2356,13 @@
         <v>6</v>
       </c>
       <c r="O29" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="P29" s="4">
         <v>44721</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -2413,16 +2400,16 @@
         <v>129</v>
       </c>
       <c r="N30" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="O30" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="P30" s="4">
         <v>44721</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -2460,10 +2447,10 @@
         <v>129</v>
       </c>
       <c r="N31" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="O31" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="P31" s="4">
         <v>44721</v>
@@ -2507,7 +2494,7 @@
         <v>6</v>
       </c>
       <c r="O32" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="P32" s="4">
         <v>44721</v>
@@ -2539,7 +2526,7 @@
         <v>2</v>
       </c>
       <c r="I33" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J33" t="s">
         <v>8</v>
@@ -2551,7 +2538,7 @@
         <v>6</v>
       </c>
       <c r="O33" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="P33" s="4">
         <v>44721</v>
@@ -2595,13 +2582,13 @@
         <v>23</v>
       </c>
       <c r="O34" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="P34" s="4">
         <v>44721</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -2624,7 +2611,7 @@
         <v>129</v>
       </c>
       <c r="N35" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="P35" s="4" t="s">
         <v>130</v>
@@ -2667,14 +2654,12 @@
       <c r="L36" t="s">
         <v>6</v>
       </c>
-      <c r="M36" t="s">
-        <v>131</v>
-      </c>
+      <c r="M36" s="5"/>
       <c r="N36" t="s">
-        <v>198</v>
+        <v>130</v>
       </c>
       <c r="O36" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="P36" s="4">
         <v>44721</v>
@@ -2706,7 +2691,7 @@
         <v>2</v>
       </c>
       <c r="I37" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J37" t="s">
         <v>8</v>
@@ -2718,7 +2703,7 @@
         <v>6</v>
       </c>
       <c r="O37" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="P37" s="4">
         <v>44721</v>
@@ -2762,7 +2747,7 @@
         <v>23</v>
       </c>
       <c r="O38" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="P38" s="4">
         <v>44721</v>
@@ -2806,13 +2791,13 @@
         <v>23</v>
       </c>
       <c r="O39" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="P39" s="4">
         <v>44721</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -2853,10 +2838,10 @@
         <v>129</v>
       </c>
       <c r="N40" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="O40" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="P40" s="4">
         <v>44721</v>
@@ -2900,13 +2885,13 @@
         <v>6</v>
       </c>
       <c r="O41" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="P41" s="4">
         <v>44721</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>71</v>
       </c>
@@ -2929,13 +2914,13 @@
         <v>129</v>
       </c>
       <c r="N42" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="P42" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -2976,10 +2961,10 @@
         <v>129</v>
       </c>
       <c r="N43" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="O43" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="P43" s="4">
         <v>44721</v>
@@ -3023,13 +3008,13 @@
         <v>6</v>
       </c>
       <c r="O44" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="P44" s="4">
         <v>44721</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>62</v>
       </c>
@@ -3070,16 +3055,16 @@
         <v>129</v>
       </c>
       <c r="N45" t="s">
-        <v>136</v>
+        <v>194</v>
       </c>
       <c r="O45" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="P45" s="4">
         <v>44721</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>72</v>
       </c>
@@ -3102,13 +3087,13 @@
         <v>129</v>
       </c>
       <c r="N46" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="P46" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>63</v>
       </c>
@@ -3149,10 +3134,10 @@
         <v>129</v>
       </c>
       <c r="N47" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O47" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="P47" s="4">
         <v>44721</v>
@@ -3196,13 +3181,13 @@
         <v>23</v>
       </c>
       <c r="O48" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="P48" s="4">
         <v>44721</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>68</v>
       </c>
@@ -3231,10 +3216,10 @@
         <v>129</v>
       </c>
       <c r="N49" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="O49" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="P49" s="4">
         <v>44721</v>
@@ -3278,13 +3263,13 @@
         <v>6</v>
       </c>
       <c r="O50" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="P50" s="4">
         <v>44721</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>73</v>
       </c>
@@ -3307,11 +3292,17 @@
         <v>129</v>
       </c>
       <c r="N51" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:M51" xr:uid="{9549FD63-5553-FE4A-95C6-DE5AEB491F85}"/>
+  <autoFilter ref="E1:M51" xr:uid="{9549FD63-5553-FE4A-95C6-DE5AEB491F85}">
+    <filterColumn colId="8">
+      <filters blank="1">
+        <filter val="TODO"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U51">
     <sortCondition ref="D2:D51"/>
   </sortState>
@@ -3332,27 +3323,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All but IA analyzed
</commit_message>
<xml_diff>
--- a/docs/WIP/Maps & Elections by State.xlsx
+++ b/docs/WIP/Maps & Elections by State.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/dev/method_eval/docs/WIP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59473D2-B9D4-0144-80D7-FB39DB1925FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0350F4D-B188-A34D-AA12-D7C5A1D64437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="500" windowWidth="27720" windowHeight="17500" xr2:uid="{681EA93E-AE60-7D46-B720-CAB4E15116B4}"/>
+    <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="17500" xr2:uid="{681EA93E-AE60-7D46-B720-CAB4E15116B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Elections by State" sheetId="2" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="197">
   <si>
     <t>AL</t>
   </si>
@@ -658,6 +658,9 @@
   </si>
   <si>
     <t>We use the regular S2018, not the special or runoff.</t>
+  </si>
+  <si>
+    <t>SWEEPS</t>
   </si>
 </sst>
 </file>
@@ -718,13 +721,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1050,7 +1052,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I37" sqref="I37"/>
+      <selection pane="bottomRight" activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1272,6 +1274,9 @@
       <c r="L5" t="s">
         <v>6</v>
       </c>
+      <c r="M5" t="s">
+        <v>196</v>
+      </c>
       <c r="O5" t="s">
         <v>181</v>
       </c>
@@ -2654,7 +2659,6 @@
       <c r="L36" t="s">
         <v>6</v>
       </c>
-      <c r="M36" s="5"/>
       <c r="N36" t="s">
         <v>130</v>
       </c>

</xml_diff>